<commit_message>
Week 5 - Re-uploaded it because 47750dc affected due to bad commit 1768c78
Signed-off-by: Synthia Islam <synthia.mist@gmail.com>
</commit_message>
<xml_diff>
--- a/Howard_S371832/TimeSheet.xlsx
+++ b/Howard_S371832/TimeSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/howardmai/Library/Mobile Documents/com~apple~CloudDocs/ACADEMY/CDU/25S2/PRT681/PRT681_S2025_developers/Howard_S371832/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921E2FA6-A302-BC42-AB97-EC060D802686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3202D76D-D9CD-3B48-9AEF-96B3DD1A5417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="33120" windowHeight="18000" xr2:uid="{BB4B9D25-F2F2-4C9B-919B-0A13ED01B91C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
   <si>
     <t>Week</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>Developed a Movie Management web app using Blazor</t>
+  </si>
+  <si>
+    <t>Learned about basic concepts of SQL, DDL, DML</t>
+  </si>
+  <si>
+    <t>Used SQL commands to create and modify schemas, databases, and tables</t>
+  </si>
+  <si>
+    <t>Learned about how to use Dapper, EF to interact with the databse</t>
   </si>
 </sst>
 </file>
@@ -439,12 +448,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -452,9 +464,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -775,8 +784,8 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1156,9 +1165,11 @@
       <c r="G27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="H27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="13"/>
       <c r="C28" s="15"/>
@@ -1168,7 +1179,9 @@
       <c r="G28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
@@ -1182,7 +1195,9 @@
       <c r="G29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
@@ -1194,20 +1209,35 @@
       <c r="G30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="3"/>
+      <c r="H30" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
+  <mergeCells count="52">
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E24"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="H10:H12"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="E9:E12"/>
@@ -1224,31 +1254,17 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E24"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="H29:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1302,14 +1318,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
@@ -1368,26 +1384,26 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -1446,36 +1462,36 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -1535,14 +1551,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="F3:F6"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="B9:B12"/>
@@ -1559,6 +1567,14 @@
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1575,12 +1591,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF7D5EB9F8E73A4CAE7C779908096F7A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e61dfdf9a683c98215621ae48838c6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d0fc1988-bccd-4bd4-9c78-560c29842df2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ced57ef6210b51da0a3f92de186c21a" ns2:_="">
     <xsd:import namespace="d0fc1988-bccd-4bd4-9c78-560c29842df2"/>
@@ -1742,6 +1752,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{458FD0F4-22B8-4D85-970B-CAC25686891E}">
   <ds:schemaRefs>
@@ -1751,15 +1767,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4455736F-9EDC-48D0-8347-108024E860C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07B82ADB-B17D-4A81-A55F-23C65B33E86E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1775,4 +1782,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4455736F-9EDC-48D0-8347-108024E860C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>